<commit_message>
refactor: move code executions into main script
</commit_message>
<xml_diff>
--- a/ayto_reality_special.xlsx
+++ b/ayto_reality_special.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lilli\git\AYTO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{644C0614-F198-4ED1-8569-5CD46926B87B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA63C34-4E05-4602-8C21-FDF5EAC9770E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1035" yWindow="1500" windowWidth="20670" windowHeight="13755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1035" yWindow="1500" windowWidth="20670" windowHeight="13755" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="matching_night_table" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="60">
   <si>
     <t>Aurelia</t>
   </si>
@@ -73,9 +73,6 @@
     <t>3</t>
   </si>
   <si>
-    <t>4, 7</t>
-  </si>
-  <si>
     <t>3, 5</t>
   </si>
   <si>
@@ -112,9 +109,6 @@
     <t>boys</t>
   </si>
   <si>
-    <t>Aurelia+Diogo</t>
-  </si>
-  <si>
     <t>Francesco</t>
   </si>
   <si>
@@ -136,15 +130,6 @@
     <t xml:space="preserve">night </t>
   </si>
   <si>
-    <t>3, 4</t>
-  </si>
-  <si>
-    <t>1, 3</t>
-  </si>
-  <si>
-    <t>1, 2, 4</t>
-  </si>
-  <si>
     <t>2, 9</t>
   </si>
   <si>
@@ -175,10 +160,49 @@
     <t>2, 3 ,4, 5, 6, 7, 8, 9</t>
   </si>
   <si>
-    <t>2, 4, 7</t>
-  </si>
-  <si>
     <t>1, 2, 5, 9</t>
+  </si>
+  <si>
+    <t>Aurelia+Josua</t>
+  </si>
+  <si>
+    <t>Finnja+Danilo</t>
+  </si>
+  <si>
+    <t>Walentina+Tommy</t>
+  </si>
+  <si>
+    <t>Melina+Tommy</t>
+  </si>
+  <si>
+    <t>Finnja+Salvo</t>
+  </si>
+  <si>
+    <t>Finnja+Eugen</t>
+  </si>
+  <si>
+    <t>Steffi+Eugen</t>
+  </si>
+  <si>
+    <t>Sarah+Josua</t>
+  </si>
+  <si>
+    <t>4, 6, 7</t>
+  </si>
+  <si>
+    <t>3, 4, 5</t>
+  </si>
+  <si>
+    <t>5, 7</t>
+  </si>
+  <si>
+    <t>2, 4, 5, 7</t>
+  </si>
+  <si>
+    <t>1, 3, 6</t>
+  </si>
+  <si>
+    <t>1, 2, 4, 5, 6</t>
   </si>
 </sst>
 </file>
@@ -570,20 +594,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -610,7 +635,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>8</v>
@@ -621,7 +646,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>10</v>
@@ -642,10 +667,10 @@
         <v>7</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J2" s="3">
         <v>1</v>
@@ -659,10 +684,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>10</v>
@@ -671,7 +696,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>10</v>
@@ -680,10 +705,10 @@
         <v>3</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J3" s="3">
         <v>0</v>
@@ -697,10 +722,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>10</v>
@@ -730,18 +755,18 @@
         <v>10</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="D5" s="2">
         <v>7</v>
@@ -765,7 +790,7 @@
         <v>0</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="L5" s="3">
         <v>0</v>
@@ -773,7 +798,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>10</v>
@@ -793,11 +818,11 @@
       <c r="G6" s="3">
         <v>0</v>
       </c>
-      <c r="H6" s="2">
-        <v>7</v>
+      <c r="H6" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="J6" s="3">
         <v>0</v>
@@ -811,13 +836,13 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>23</v>
+      </c>
+      <c r="B7" s="2">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>10</v>
@@ -832,7 +857,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>10</v>
@@ -841,7 +866,7 @@
         <v>0</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="L7" s="3">
         <v>8</v>
@@ -849,7 +874,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>10</v>
@@ -864,7 +889,7 @@
         <v>14</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -887,7 +912,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>10</v>
@@ -896,7 +921,7 @@
         <v>10</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E9" s="2">
         <v>7</v>
@@ -917,7 +942,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="L9" s="3">
         <v>0</v>
@@ -925,7 +950,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>10</v>
@@ -952,7 +977,7 @@
         <v>10</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>10</v>
@@ -963,13 +988,13 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>10</v>
@@ -981,7 +1006,7 @@
         <v>10</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>10</v>
@@ -1082,20 +1107,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7A0AB78-603E-4E95-8C56-F8768DD5F405}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1103,7 +1131,15 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1113,28 +1149,79 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED8DB9CD-5432-4BF4-968A-68819B3C4F5F}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
-        <v>29</v>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>